<commit_message>
add prior year department
</commit_message>
<xml_diff>
--- a/STAFF_REPORT.xlsx
+++ b/STAFF_REPORT.xlsx
@@ -600,21 +600,21 @@
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>2</t>
         </is>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="S2" t="n">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="T2" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
@@ -678,21 +678,21 @@
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>2</t>
         </is>
       </c>
       <c r="R3" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="S3" t="n">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
@@ -756,21 +756,21 @@
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>asdf</t>
+          <t>2</t>
         </is>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="S4" t="n">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="T4" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>